<commit_message>
add convert xml json to nosql or JsonNode
</commit_message>
<xml_diff>
--- a/dataset/data.xlsx
+++ b/dataset/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work station\ProjectDigio\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work station\git\BatchSystem\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6694701-772E-419B-9C81-FBDBD51E30A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A18353-276C-4B13-8406-BA39AED18984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3120" windowWidth="25770" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="4185" windowWidth="25770" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,7 +387,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +414,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>

</xml_diff>